<commit_message>
Primul raport pe Requirement Tasks.
</commit_message>
<xml_diff>
--- a/Docs/Evaluare/Lab01_ReviewReport.xlsx
+++ b/Docs/Evaluare/Lab01_ReviewReport.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VVSS\01_Tasks\Docs\Evaluare\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B34C72A6-579B-4B7F-BB0A-8865C35E26BA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="156" windowWidth="14160" windowHeight="8268" tabRatio="650" activeTab="3"/>
+    <workbookView xWindow="5568" yWindow="0" windowWidth="17280" windowHeight="9060" tabRatio="650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements Phase Defects" sheetId="7" r:id="rId1"/>
@@ -12,12 +18,15 @@
     <sheet name="Coding Phase Defects" sheetId="5" r:id="rId3"/>
     <sheet name="Tool-basedCodeAnalysis" sheetId="8" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Requirements Phase Defects'!$B$9:$E$30</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="75">
   <si>
     <t>Document  Title:</t>
   </si>
@@ -116,12 +125,138 @@
   </si>
   <si>
     <t>Effort to perform tool-based code analysis (hours):</t>
+  </si>
+  <si>
+    <t>Punga Alexandru</t>
+  </si>
+  <si>
+    <t>Suciu Alexandra</t>
+  </si>
+  <si>
+    <t>Vasilcovschi Tudor Constantin</t>
+  </si>
+  <si>
+    <t>R01</t>
+  </si>
+  <si>
+    <t>R02</t>
+  </si>
+  <si>
+    <t>R04</t>
+  </si>
+  <si>
+    <t>R05</t>
+  </si>
+  <si>
+    <t>R06</t>
+  </si>
+  <si>
+    <t>R07</t>
+  </si>
+  <si>
+    <t>F01</t>
+  </si>
+  <si>
+    <t>01.Tasks</t>
+  </si>
+  <si>
+    <t>Precizarea formatul in care sunt salvate datele in fisiere</t>
+  </si>
+  <si>
+    <t>Task-ul ar trebui sa contina un status</t>
+  </si>
+  <si>
+    <t>F05</t>
+  </si>
+  <si>
+    <t>Forma de identificare</t>
+  </si>
+  <si>
+    <t>Nu se precizeaza faptul ca trebuie sa contina un ID</t>
+  </si>
+  <si>
+    <t>F04</t>
+  </si>
+  <si>
+    <t>F03</t>
+  </si>
+  <si>
+    <t>Forma de identificare a task-ului afisat</t>
+  </si>
+  <si>
+    <t>F02</t>
+  </si>
+  <si>
+    <t>Ordinea nu este precizata</t>
+  </si>
+  <si>
+    <t>Nu se precizeaza limbajul in care se va dezvolta aplicatia</t>
+  </si>
+  <si>
+    <t>Nu se precizeaza pentru ce platforma se va dezvolta aplicatia</t>
+  </si>
+  <si>
+    <t>R02/R04</t>
+  </si>
+  <si>
+    <t>F02/F03</t>
+  </si>
+  <si>
+    <t>R02/R05</t>
+  </si>
+  <si>
+    <t>Nu se specifica unde/cum se afiseaza datele</t>
+  </si>
+  <si>
+    <t>F06</t>
+  </si>
+  <si>
+    <t>Nu se specifica citirea/scriere din/in fisier ca Feature</t>
+  </si>
+  <si>
+    <t>F05/F04/F02</t>
+  </si>
+  <si>
+    <t>La stergerea/modificarea unui task se sterge/modifica pentru toate repetitiile acestuia?</t>
+  </si>
+  <si>
+    <t>Formatul datei si orei in fisier</t>
+  </si>
+  <si>
+    <t>Se foloseste interfata grafica/consola?</t>
+  </si>
+  <si>
+    <t>01.Tasks/F03/F02</t>
+  </si>
+  <si>
+    <t>Toata task-urile/doar cele active/doar cele inactive</t>
+  </si>
+  <si>
+    <t>Ce se intampla cand user-ul iese din aplicatie?</t>
+  </si>
+  <si>
+    <t>F01/F04/F05</t>
+  </si>
+  <si>
+    <t>Necesita logare</t>
+  </si>
+  <si>
+    <t>Nu se specifica daca la finalul task-ului acesta devine inactiv/se sterge</t>
+  </si>
+  <si>
+    <t>Ce campuri se pot modifica</t>
+  </si>
+  <si>
+    <t>F05/F01/F02</t>
+  </si>
+  <si>
+    <t>Inquisitors</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -194,7 +329,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -216,6 +351,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -293,7 +434,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -315,9 +456,6 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -365,6 +503,21 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -374,6 +527,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -422,7 +578,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -455,9 +611,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -490,6 +663,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -665,105 +855,121 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor theme="7" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A1:J27"/>
+  <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.89453125" style="6"/>
-    <col min="2" max="2" width="12.3125" style="6" customWidth="1"/>
-    <col min="3" max="4" width="16.3125" style="6" customWidth="1"/>
-    <col min="5" max="5" width="41.41796875" style="6" customWidth="1"/>
-    <col min="6" max="8" width="8.89453125" style="6"/>
-    <col min="9" max="9" width="21" style="6" customWidth="1"/>
-    <col min="10" max="10" width="14.41796875" style="6" customWidth="1"/>
-    <col min="11" max="16384" width="8.89453125" style="6"/>
+    <col min="1" max="1" width="8.88671875" style="6"/>
+    <col min="2" max="2" width="12.33203125" style="6" customWidth="1"/>
+    <col min="3" max="4" width="16.33203125" style="6" customWidth="1"/>
+    <col min="5" max="5" width="41.44140625" style="6" customWidth="1"/>
+    <col min="6" max="8" width="8.88671875" style="6"/>
+    <col min="9" max="9" width="25.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.44140625" style="6" customWidth="1"/>
+    <col min="11" max="16384" width="8.88671875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="22" t="s">
+      <c r="H1" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="B2" s="23" t="s">
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B2" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
       <c r="H2" s="3"/>
-      <c r="I2" s="20" t="s">
+      <c r="I2" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="J2" s="18" t="s">
+      <c r="J2" s="17" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="H3" s="18" t="s">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="H3" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="18"/>
-      <c r="J3" s="18"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="I3" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="J3" s="17">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C4" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="24" t="s">
+      <c r="D4" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="24"/>
-      <c r="H4" s="18" t="s">
+      <c r="E4" s="23"/>
+      <c r="H4" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="I4" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="J4" s="3">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C5" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="25" t="s">
+      <c r="D5" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="26"/>
-      <c r="H5" s="18" t="s">
+      <c r="E5" s="25"/>
+      <c r="H5" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="I5" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="J5" s="3">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="D6" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="E6" s="20"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="D7" s="40">
+        <v>44250</v>
+      </c>
+      <c r="E7" s="20"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
@@ -777,160 +983,324 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B10" s="3">
         <v>1</v>
       </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="2"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="C10" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="2"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="C11" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B12" s="3">
-        <f t="shared" ref="B12:B25" si="0">B11+1</f>
+        <f>B11+1</f>
         <v>3</v>
       </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="2"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="C12" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="E12" s="34" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B13" s="3">
-        <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="2"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="B14" s="3">
-        <f t="shared" si="0"/>
+      <c r="C13" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B14" s="35">
+        <f>B13+1</f>
         <v>5</v>
       </c>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="2"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="C14" s="36" t="s">
+        <v>37</v>
+      </c>
+      <c r="D14" s="36" t="s">
+        <v>43</v>
+      </c>
+      <c r="E14" s="37" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B15" s="3">
-        <f t="shared" si="0"/>
+        <f>B14+1</f>
         <v>6</v>
       </c>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="2"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="C15" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="D15" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="E15" s="34" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B16" s="3">
-        <f t="shared" si="0"/>
+        <f>B15+1</f>
         <v>7</v>
       </c>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="2"/>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="B17" s="3">
-        <f t="shared" si="0"/>
+      <c r="C16" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="D16" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="E16" s="34" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B17" s="35">
+        <f>B16+1</f>
         <v>8</v>
       </c>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="2"/>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="C17" s="38" t="s">
+        <v>37</v>
+      </c>
+      <c r="D17" s="38" t="s">
+        <v>42</v>
+      </c>
+      <c r="E17" s="39" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B18" s="3">
-        <f t="shared" si="0"/>
+        <f>B17+1</f>
         <v>9</v>
       </c>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="16"/>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="C18" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="D18" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="E18" s="34" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B19" s="3">
-        <f t="shared" si="0"/>
+        <f>B18+1</f>
         <v>10</v>
       </c>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="16"/>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="C19" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="D19" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="E19" s="34" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B20" s="3">
-        <f t="shared" si="0"/>
+        <f>B19+1</f>
         <v>11</v>
       </c>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="16"/>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="C20" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="D20" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="E20" s="34" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B21" s="3">
-        <f t="shared" si="0"/>
+        <f>B20+1</f>
         <v>12</v>
       </c>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="16"/>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="C21" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="D21" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="E21" s="34" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B22" s="3">
-        <f t="shared" si="0"/>
+        <f>B21+1</f>
         <v>13</v>
       </c>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="16"/>
-    </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="C22" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B23" s="3">
-        <f t="shared" si="0"/>
+        <f>B22+1</f>
         <v>14</v>
       </c>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="16"/>
-    </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="C23" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B24" s="3">
-        <f t="shared" si="0"/>
+        <f>B23+1</f>
         <v>15</v>
       </c>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="16"/>
-    </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="C24" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="D24" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="E24" s="34" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B25" s="3">
-        <f t="shared" si="0"/>
+        <f>B24+1</f>
         <v>16</v>
       </c>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="16"/>
-    </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="E26" s="11"/>
-    </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="C27" s="12" t="s">
+      <c r="C25" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="D25" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="E25" s="34" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B26" s="3">
+        <v>17</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B27" s="3">
+        <v>18</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B28" s="3">
+        <f>B27+1</f>
+        <v>19</v>
+      </c>
+      <c r="C28" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="D28" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="E28" s="34" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B29" s="3">
+        <f>B28+1</f>
+        <v>20</v>
+      </c>
+      <c r="C29" s="19"/>
+      <c r="D29" s="19"/>
+      <c r="E29" s="34"/>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B30" s="3">
+        <f>B29+1</f>
+        <v>21</v>
+      </c>
+      <c r="C30" s="19"/>
+      <c r="D30" s="19"/>
+      <c r="E30" s="34"/>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B31" s="3"/>
+      <c r="E31" s="11"/>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C32" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="D27" s="13"/>
-      <c r="E27" s="1"/>
+      <c r="D32" s="13"/>
+      <c r="E32" s="1">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
+  <autoFilter ref="B9:E30" xr:uid="{E237BE76-13B8-4525-89CA-4239F567C81A}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B10:E30">
+      <sortCondition ref="C9:C30"/>
+    </sortState>
+  </autoFilter>
   <mergeCells count="6">
     <mergeCell ref="D7:E7"/>
     <mergeCell ref="H1:J1"/>
@@ -945,104 +1315,116 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor theme="9" tint="0.59999389629810485"/>
   </sheetPr>
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H1" sqref="H1:J5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.89453125" style="6"/>
-    <col min="2" max="2" width="12.3125" style="6" customWidth="1"/>
-    <col min="3" max="4" width="16.3125" style="6" customWidth="1"/>
-    <col min="5" max="5" width="41.41796875" style="6" customWidth="1"/>
-    <col min="6" max="8" width="8.89453125" style="6"/>
-    <col min="9" max="9" width="22.05078125" style="6" customWidth="1"/>
-    <col min="10" max="16384" width="8.89453125" style="6"/>
+    <col min="1" max="1" width="8.88671875" style="6"/>
+    <col min="2" max="2" width="12.33203125" style="6" customWidth="1"/>
+    <col min="3" max="4" width="16.33203125" style="6" customWidth="1"/>
+    <col min="5" max="5" width="41.44140625" style="6" customWidth="1"/>
+    <col min="6" max="8" width="8.88671875" style="6"/>
+    <col min="9" max="9" width="25.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.88671875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="22" t="s">
+      <c r="H1" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="B2" s="23" t="s">
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B2" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
       <c r="H2" s="3"/>
-      <c r="I2" s="20" t="s">
+      <c r="I2" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="J2" s="18" t="s">
+      <c r="J2" s="17" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="H3" s="18" t="s">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="H3" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="18"/>
-      <c r="J3" s="18"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="I3" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="J3" s="17">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C4" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="27" t="s">
+      <c r="D4" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="27"/>
-      <c r="H4" s="18" t="s">
+      <c r="E4" s="26"/>
+      <c r="H4" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="I4" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="J4" s="3">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C5" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="28" t="s">
+      <c r="D5" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="29"/>
-      <c r="H5" s="18" t="s">
+      <c r="E5" s="28"/>
+      <c r="H5" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="I5" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="J5" s="3">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
@@ -1056,7 +1438,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B10" s="3">
         <v>1</v>
       </c>
@@ -1064,7 +1446,7 @@
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
@@ -1073,7 +1455,7 @@
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B26" si="0">B11+1</f>
         <v>3</v>
@@ -1082,7 +1464,7 @@
       <c r="D12" s="1"/>
       <c r="E12" s="2"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1091,7 +1473,7 @@
       <c r="D13" s="1"/>
       <c r="E13" s="2"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1100,7 +1482,7 @@
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1109,7 +1491,7 @@
       <c r="D15" s="1"/>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1118,7 +1500,7 @@
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1127,7 +1509,7 @@
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1136,7 +1518,7 @@
       <c r="D18" s="1"/>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1145,7 +1527,7 @@
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1154,7 +1536,7 @@
       <c r="D20" s="1"/>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1163,7 +1545,7 @@
       <c r="D21" s="1"/>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1172,7 +1554,7 @@
       <c r="D22" s="1"/>
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1181,7 +1563,7 @@
       <c r="D23" s="1"/>
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1190,7 +1572,7 @@
       <c r="D24" s="1"/>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1199,7 +1581,7 @@
       <c r="D25" s="1"/>
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B26" s="3">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1208,10 +1590,10 @@
       <c r="D26" s="1"/>
       <c r="E26" s="2"/>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
       <c r="E27" s="11"/>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C28" s="12" t="s">
         <v>8</v>
       </c>
@@ -1233,105 +1615,117 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor theme="3" tint="0.59999389629810485"/>
   </sheetPr>
   <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="H1" sqref="H1:J5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.89453125" style="6"/>
-    <col min="2" max="2" width="12.3125" style="6" customWidth="1"/>
-    <col min="3" max="3" width="16.3125" style="6" customWidth="1"/>
+    <col min="1" max="1" width="8.88671875" style="6"/>
+    <col min="2" max="2" width="12.33203125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" style="6" customWidth="1"/>
     <col min="4" max="4" width="18" style="6" customWidth="1"/>
-    <col min="5" max="5" width="41.41796875" style="6" customWidth="1"/>
-    <col min="6" max="8" width="8.89453125" style="6"/>
-    <col min="9" max="9" width="26.734375" style="6" customWidth="1"/>
-    <col min="10" max="16384" width="8.89453125" style="6"/>
+    <col min="5" max="5" width="41.44140625" style="6" customWidth="1"/>
+    <col min="6" max="8" width="8.88671875" style="6"/>
+    <col min="9" max="9" width="25.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.88671875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="22" t="s">
+      <c r="H1" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="B2" s="23" t="s">
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B2" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
       <c r="H2" s="3"/>
-      <c r="I2" s="20" t="s">
+      <c r="I2" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="J2" s="18" t="s">
+      <c r="J2" s="17" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="H3" s="18" t="s">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="H3" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="18"/>
-      <c r="J3" s="18"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="C4" s="17" t="s">
+      <c r="I3" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="J3" s="17">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C4" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="30" t="s">
+      <c r="D4" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="30"/>
-      <c r="H4" s="18" t="s">
+      <c r="E4" s="29"/>
+      <c r="H4" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="C5" s="17" t="s">
+      <c r="I4" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="J4" s="3">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C5" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="31" t="s">
+      <c r="D5" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="32"/>
-      <c r="H5" s="18" t="s">
+      <c r="E5" s="31"/>
+      <c r="H5" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="I5" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="J5" s="3">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
@@ -1345,7 +1739,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B10" s="3">
         <v>1</v>
       </c>
@@ -1353,7 +1747,7 @@
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
@@ -1362,7 +1756,7 @@
       <c r="D11" s="1"/>
       <c r="E11" s="2"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B30" si="0">B11+1</f>
         <v>3</v>
@@ -1371,7 +1765,7 @@
       <c r="D12" s="1"/>
       <c r="E12" s="2"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1380,7 +1774,7 @@
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1389,7 +1783,7 @@
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1398,7 +1792,7 @@
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1407,7 +1801,7 @@
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1416,7 +1810,7 @@
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1425,7 +1819,7 @@
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1434,7 +1828,7 @@
       <c r="D19" s="1"/>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1443,7 +1837,7 @@
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1452,7 +1846,7 @@
       <c r="D21" s="1"/>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1461,7 +1855,7 @@
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1470,7 +1864,7 @@
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1479,7 +1873,7 @@
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1488,7 +1882,7 @@
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B26" s="3">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1497,7 +1891,7 @@
       <c r="D26" s="1"/>
       <c r="E26" s="2"/>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B27" s="3">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -1506,7 +1900,7 @@
       <c r="D27" s="2"/>
       <c r="E27" s="1"/>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B28" s="3">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -1515,7 +1909,7 @@
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B29" s="3">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -1524,7 +1918,7 @@
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B30" s="3">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -1533,10 +1927,10 @@
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="2:5" x14ac:dyDescent="0.3">
       <c r="E31" s="11"/>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C32" s="12" t="s">
         <v>8</v>
       </c>
@@ -1558,95 +1952,107 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <tabColor theme="6" tint="0.79998168889431442"/>
   </sheetPr>
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H1" sqref="H1:J5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.89453125" style="6"/>
-    <col min="2" max="2" width="12.3125" style="6" customWidth="1"/>
-    <col min="3" max="3" width="16.3125" style="6" customWidth="1"/>
+    <col min="1" max="1" width="8.88671875" style="6"/>
+    <col min="2" max="2" width="12.33203125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" style="6" customWidth="1"/>
     <col min="4" max="4" width="18" style="6" customWidth="1"/>
-    <col min="5" max="5" width="23.9453125" style="6" customWidth="1"/>
-    <col min="6" max="6" width="16.62890625" style="6" customWidth="1"/>
-    <col min="7" max="8" width="8.89453125" style="6"/>
-    <col min="9" max="9" width="26.734375" style="6" customWidth="1"/>
-    <col min="10" max="16384" width="8.89453125" style="6"/>
+    <col min="5" max="5" width="24" style="6" customWidth="1"/>
+    <col min="6" max="6" width="16.6640625" style="6" customWidth="1"/>
+    <col min="7" max="8" width="8.88671875" style="6"/>
+    <col min="9" max="9" width="25.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.88671875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="22" t="s">
+      <c r="H1" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="B2" s="23" t="s">
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B2" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
       <c r="H2" s="3"/>
-      <c r="I2" s="20" t="s">
+      <c r="I2" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="J2" s="18" t="s">
+      <c r="J2" s="17" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="H3" s="18" t="s">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="H3" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="18"/>
-      <c r="J3" s="18"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="C4" s="17" t="s">
+      <c r="I3" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="J3" s="17">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C4" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
-      <c r="H4" s="18" t="s">
+      <c r="D4" s="29"/>
+      <c r="E4" s="29"/>
+      <c r="H4" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="I4" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="J4" s="3">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C5" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="H5" s="18" t="s">
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
+      <c r="H5" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="I5" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="J5" s="3">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
@@ -1663,7 +2069,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B10" s="3">
         <v>1</v>
       </c>
@@ -1672,7 +2078,7 @@
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
@@ -1682,7 +2088,7 @@
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B30" si="0">B11+1</f>
         <v>3</v>
@@ -1692,7 +2098,7 @@
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1702,7 +2108,7 @@
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1712,7 +2118,7 @@
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1722,7 +2128,7 @@
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1732,7 +2138,7 @@
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1742,7 +2148,7 @@
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1752,7 +2158,7 @@
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1762,7 +2168,7 @@
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1772,7 +2178,7 @@
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1782,7 +2188,7 @@
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1792,7 +2198,7 @@
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1802,7 +2208,7 @@
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1812,7 +2218,7 @@
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1822,7 +2228,7 @@
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B26" s="3">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1832,7 +2238,7 @@
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B27" s="3">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -1842,7 +2248,7 @@
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B28" s="3">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -1852,7 +2258,7 @@
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B29" s="3">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -1862,7 +2268,7 @@
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B30" s="3">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -1872,16 +2278,16 @@
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
     </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="2:6" x14ac:dyDescent="0.3">
       <c r="E31" s="11"/>
     </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="C32" s="33" t="s">
+    <row r="32" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C32" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="D32" s="34"/>
-      <c r="E32" s="34"/>
-      <c r="F32" s="19"/>
+      <c r="D32" s="33"/>
+      <c r="E32" s="33"/>
+      <c r="F32" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>